<commit_message>
Update formula field in worktime Update excel output column position in worktime-template.xls Throw exception in worktime batch update because formula override issue.
</commit_message>
<xml_diff>
--- a/src/main/resources/excel-template/worktime-template.xlsx
+++ b/src/main/resources/excel-template/worktime-template.xlsx
@@ -530,14 +530,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>${worktime.bwAvgViews.0.assyAvg}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>${worktime.bwAvgViews.0.packingAvg}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>w</t>
     </r>
@@ -587,6 +579,14 @@
       </rPr>
       <t>Name</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>${worktime.bwFields.0.assyAvg}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>${worktime.bwFields.0.packingAvg}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BI2" sqref="BI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -988,10 +988,10 @@
         <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>12</v>
@@ -1162,7 +1162,7 @@
         <v>111</v>
       </c>
       <c r="BJ1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="15.75" x14ac:dyDescent="0.2">
@@ -1176,10 +1176,10 @@
         <v>56</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -1344,13 +1344,13 @@
         <v>112</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>

</xml_diff>